<commit_message>
Added some Expense information
</commit_message>
<xml_diff>
--- a/Documents/Expense Report.xlsx
+++ b/Documents/Expense Report.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Date:</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>Expense/Time:</t>
+  </si>
+  <si>
+    <t>$10.90/year</t>
+  </si>
+  <si>
+    <t>Business Cards (250 for advertising and clients)</t>
   </si>
 </sst>
 </file>
@@ -483,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -553,6 +559,20 @@
         <v>6</v>
       </c>
     </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="4">
+        <v>41662</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>